<commit_message>
updated bom for rfof enclosure
</commit_message>
<xml_diff>
--- a/Analog-Signal-Components/RFoF/1U-Enclosure/Sourcing_RFoF_Enclosure.xlsx
+++ b/Analog-Signal-Components/RFoF/1U-Enclosure/Sourcing_RFoF_Enclosure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pollak/Documents/GitHub/Front-Page/Analog-Signal-Components/2025-RFoF/1U-Enclosure/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colin\Documents\ATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8185D26E-4899-0948-A88B-E3C6967796E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48DEDCD-243E-4930-BA39-D86A0F9F5B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-99480" yWindow="1000" windowWidth="30220" windowHeight="21560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2625" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="145">
   <si>
     <t>Name</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Datasheet</t>
   </si>
   <si>
-    <t>Standoffs</t>
-  </si>
-  <si>
     <t>Linear PSU</t>
   </si>
   <si>
@@ -125,21 +122,12 @@
     <t>https://www.minicircuits.com/pdfs/SF-SF50+.pdf</t>
   </si>
   <si>
-    <t>M2.5 Standoff Assortment Brass</t>
-  </si>
-  <si>
     <t>M2.5 assortment</t>
   </si>
   <si>
-    <t>helifouner</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>https://www.amazon.com/HELIFOUNER-Standoffs-Assortment-Threaded-Motherboard/dp/B0B7SNCFF1/ref=sr_1_1_sspa?s=industrial&amp;sr=1-1-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9hdGY</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
@@ -398,9 +386,6 @@
     <t>https://resource.fs.com/mall/resource/fc-apc-simplex-metal-fiber-optic-adapter-datasheet.pdf</t>
   </si>
   <si>
-    <t>M3 8mm Screws</t>
-  </si>
-  <si>
     <t>https://www.mcmaster.com/products/screws/system-of-measurement~metric/thread-size~m3/length~8-mm/rounded-head-screws-2~/metric-18-8-stainless-steel-pan-head-phillips-screws/</t>
   </si>
   <si>
@@ -408,13 +393,91 @@
   </si>
   <si>
     <t>McMaster-Carr</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Apem/Q6F3CXXR02E?qs=4pzlT8jjbheF1OmuiSn%2Fng%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/catalog/specsheets/Apem_09152017_Q6.pdf</t>
+  </si>
+  <si>
+    <t>Q6F3GXXR02E</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Alamic-Silicone-Waterproof-Sealing-Diameter/dp/B0D573DQP7?th=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Kindroufly-Pieces-Countersunk-Washers-Assortment/dp/B0BLCG712G/ref=sr_1_2?crid=1595QJHI4TJZT&amp;dib=eyJ2IjoiMSJ9.sebXe-wj3Kw9IjP28AlXbKFqjftUpWI7gaLXU-S-oY-XjgIbeZKYhpHMilN1UR7Tbsj0DhHKFVfsP1_Lby1GNxAKx6AHy-foBx5XZU2Q2WLY4v5EeXi_9ndunPhL4urxaLg84EVJrZh_BPvjLMMvs50HJUOKvFWT-uFZm2yQwNvBlTjaqmC79h3LyQJig6ejBdeE-x_ileQSDuG47rMZhi7Blouj0XbZEtYVK69Kc1lvdC62vDEVhpYihA8rWBYRmWMBpaFd6n9QBgfvSgNjhYaUcMt3zeQbcJbogaUw9Kk.5ZLxw2KOhNwAjNDfBS3qB9GG7t6Pm_u4uGA-HjHmobA&amp;dib_tag=se&amp;keywords=kindroufly%2B562%2Bm2.5%2Bcountersunk%2Bhead&amp;qid=1766091235&amp;s=industrial&amp;sprefix=kindroufly%2B562%2Bm2.5%2Bcountersunk%2Bhead%2Cindustrial%2C128&amp;sr=1-2&amp;th=1</t>
+  </si>
+  <si>
+    <t>M2.5 Button Head</t>
+  </si>
+  <si>
+    <t>M2.5 Countersunk</t>
+  </si>
+  <si>
+    <t>M2.5 Countersunk screw assortment</t>
+  </si>
+  <si>
+    <t>Silicone LED plugs</t>
+  </si>
+  <si>
+    <t>6mm Silicone plugs for empty LED slots</t>
+  </si>
+  <si>
+    <t>Alamic</t>
+  </si>
+  <si>
+    <t>WNSPK</t>
+  </si>
+  <si>
+    <t>SMA Cable</t>
+  </si>
+  <si>
+    <t>Hand-Flex Interconnect, 0.086" center diameter, 18.0 GHz, 14.0″</t>
+  </si>
+  <si>
+    <t>086-14SM+</t>
+  </si>
+  <si>
+    <t>https://www.minicircuits.com/WebStore/dashboard.html?model=086-14SM%2B</t>
+  </si>
+  <si>
+    <t>https://www.minicircuits.com/pdfs/086-14SM+.pdf</t>
+  </si>
+  <si>
+    <t>Cable</t>
+  </si>
+  <si>
+    <t>Panelmount</t>
+  </si>
+  <si>
+    <t>M3x8 Pan Head</t>
+  </si>
+  <si>
+    <t>M4x14 Button Head</t>
+  </si>
+  <si>
+    <t>Stainless Steel Button Head Hex-Drive Screws</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/products/screws/rounded-head-screws-2~/thread-size~m4-1/length~14-mm/</t>
+  </si>
+  <si>
+    <t>Front Panel</t>
+  </si>
+  <si>
+    <t>Interior Components</t>
+  </si>
+  <si>
+    <t>Power</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,16 +521,36 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -484,12 +567,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -507,6 +599,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -788,655 +884,816 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="34.33203125" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" t="s">
         <v>86</v>
       </c>
-      <c r="C5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E5" t="s">
-        <v>90</v>
-      </c>
       <c r="F5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G10" t="s">
+        <v>119</v>
+      </c>
+      <c r="H10" t="s">
+        <v>120</v>
+      </c>
+      <c r="I10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
         <v>90</v>
       </c>
-      <c r="F6" t="s">
+      <c r="C11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" t="s">
         <v>92</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="F11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11" t="s">
+        <v>95</v>
+      </c>
+      <c r="I11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F11" t="s">
-        <v>76</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="I11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>2</v>
-      </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>127</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>128</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>23</v>
+        <v>129</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="H12" t="s">
+        <v>30</v>
       </c>
       <c r="I12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
       <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D13" t="s">
         <v>25</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="I13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" t="s">
+        <v>137</v>
+      </c>
+      <c r="E14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F14" t="s">
+        <v>113</v>
+      </c>
+      <c r="G14" t="s">
+        <v>114</v>
+      </c>
+      <c r="H14" t="s">
+        <v>115</v>
+      </c>
+      <c r="I14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" t="s">
         <v>100</v>
       </c>
-      <c r="C14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="I14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>51</v>
-      </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>101</v>
       </c>
       <c r="E17" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="F17" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>34</v>
+        <v>103</v>
+      </c>
+      <c r="G17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H17" t="s">
+        <v>105</v>
       </c>
       <c r="I17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" t="s">
-        <v>41</v>
+        <v>107</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>136</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>108</v>
       </c>
       <c r="F18" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>34</v>
+        <v>109</v>
+      </c>
+      <c r="G18" t="s">
+        <v>110</v>
       </c>
       <c r="I18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>102</v>
+        <v>19</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="E19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E20" t="s">
-        <v>96</v>
+        <v>39</v>
       </c>
       <c r="F20" t="s">
-        <v>95</v>
-      </c>
-      <c r="G20" t="s">
-        <v>98</v>
-      </c>
-      <c r="H20" t="s">
-        <v>99</v>
+        <v>29</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="I20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="D21" t="s">
-        <v>105</v>
+        <v>136</v>
       </c>
       <c r="E21" t="s">
-        <v>106</v>
+        <v>17</v>
       </c>
       <c r="F21" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="G21" t="s">
-        <v>108</v>
+        <v>134</v>
       </c>
       <c r="H21" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="I21" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>2</v>
-      </c>
-      <c r="B22" t="s">
-        <v>111</v>
-      </c>
-      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E22" t="s">
-        <v>112</v>
-      </c>
-      <c r="F22" t="s">
-        <v>113</v>
-      </c>
-      <c r="G22" t="s">
-        <v>114</v>
-      </c>
-      <c r="I22" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>2</v>
-      </c>
-      <c r="B23" t="s">
-        <v>115</v>
-      </c>
-      <c r="C23" t="s">
-        <v>116</v>
-      </c>
-      <c r="D23" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" t="s">
-        <v>112</v>
-      </c>
-      <c r="F23" t="s">
-        <v>117</v>
-      </c>
-      <c r="G23" t="s">
-        <v>118</v>
-      </c>
-      <c r="H23" t="s">
-        <v>119</v>
-      </c>
-      <c r="I23" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C24" t="s">
-        <v>122</v>
+        <v>33</v>
+      </c>
+      <c r="D24" t="s">
+        <v>28</v>
       </c>
       <c r="E24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" t="s">
+        <v>117</v>
+      </c>
+      <c r="D25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" t="s">
+        <v>116</v>
+      </c>
+      <c r="H25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I25" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" t="s">
+        <v>126</v>
+      </c>
+      <c r="D26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G24" t="s">
-        <v>121</v>
-      </c>
-      <c r="I24" t="s">
-        <v>123</v>
+      <c r="H26" t="s">
+        <v>30</v>
+      </c>
+      <c r="I26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>139</v>
+      </c>
+      <c r="C27" t="s">
+        <v>140</v>
+      </c>
+      <c r="D27" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" t="s">
+        <v>118</v>
+      </c>
+      <c r="F27" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" t="s">
+        <v>141</v>
+      </c>
+      <c r="H27" t="s">
+        <v>30</v>
+      </c>
+      <c r="I27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" t="s">
+        <v>52</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" t="s">
+        <v>58</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" t="s">
+        <v>68</v>
+      </c>
+      <c r="F34" t="s">
+        <v>72</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I35" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H7" r:id="rId1" xr:uid="{B2FBBAF7-134D-4FB4-AEDF-1EE021FED514}"/>
-    <hyperlink ref="G7" r:id="rId2" xr:uid="{75E3293B-506B-4579-9237-00CD51655B0E}"/>
-    <hyperlink ref="H12" r:id="rId3" xr:uid="{80975C0B-98ED-4D63-8D7D-ABECCC557284}"/>
-    <hyperlink ref="G12" r:id="rId4" xr:uid="{5FB77BB6-DAD7-45E3-A834-A6FA1AA8DF56}"/>
-    <hyperlink ref="G14" r:id="rId5" xr:uid="{2637BFFD-C1B7-42C5-912C-11370728195A}"/>
-    <hyperlink ref="H8" r:id="rId6" xr:uid="{93B9BFE8-38CE-45C5-9031-E59748832B39}"/>
-    <hyperlink ref="G18" r:id="rId7" xr:uid="{748CA803-0FC4-4025-91EA-6BB94D883F0A}"/>
+    <hyperlink ref="H30" r:id="rId1" xr:uid="{B2FBBAF7-134D-4FB4-AEDF-1EE021FED514}"/>
+    <hyperlink ref="G30" r:id="rId2" xr:uid="{75E3293B-506B-4579-9237-00CD51655B0E}"/>
+    <hyperlink ref="H19" r:id="rId3" xr:uid="{80975C0B-98ED-4D63-8D7D-ABECCC557284}"/>
+    <hyperlink ref="G19" r:id="rId4" xr:uid="{5FB77BB6-DAD7-45E3-A834-A6FA1AA8DF56}"/>
+    <hyperlink ref="G9" r:id="rId5" xr:uid="{2637BFFD-C1B7-42C5-912C-11370728195A}"/>
+    <hyperlink ref="H31" r:id="rId6" xr:uid="{93B9BFE8-38CE-45C5-9031-E59748832B39}"/>
+    <hyperlink ref="G20" r:id="rId7" xr:uid="{748CA803-0FC4-4025-91EA-6BB94D883F0A}"/>
     <hyperlink ref="H4" r:id="rId8" xr:uid="{D73A4ACF-AF46-489B-81A5-6F0DD1D1BD64}"/>
     <hyperlink ref="G4" r:id="rId9" xr:uid="{F06FB6EA-9C3F-4E93-A5D7-AD3D7192D5C2}"/>
-    <hyperlink ref="G15" r:id="rId10" xr:uid="{1A3E13A5-397E-4680-BE04-43EA94453D15}"/>
-    <hyperlink ref="G16" r:id="rId11" xr:uid="{A51026F3-9695-40CA-9685-7F309BE91CAA}"/>
-    <hyperlink ref="G17" r:id="rId12" xr:uid="{F586C697-E2BF-4983-A460-646CACB8B04C}"/>
+    <hyperlink ref="G24" r:id="rId10" xr:uid="{A51026F3-9695-40CA-9685-7F309BE91CAA}"/>
+    <hyperlink ref="G35" r:id="rId11" xr:uid="{F586C697-E2BF-4983-A460-646CACB8B04C}"/>
+    <hyperlink ref="G12" r:id="rId12" xr:uid="{90C0915E-24A4-410D-8681-49A0E4C3DF9A}"/>
+    <hyperlink ref="G26" r:id="rId13" display="https://www.amazon.com/Alamic-Silicone-Waterproof-Sealing-Diameter/dp/B0D573DQP7?th=1" xr:uid="{E8E5566D-3067-40E2-838F-3D1FA2898EAA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>